<commit_message>
Updated code to parse 120 data
</commit_message>
<xml_diff>
--- a/tokopedia_scrapperIntel Core i5.xlsx
+++ b/tokopedia_scrapperIntel Core i5.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,28 +473,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>LAPTOP AXIOO MYBOOK HYPE 5 (G12) BLACK :  INTEL CORE I5-1235U 8GB 256GBSSD WIN11 (SLEVCASE)</t>
+          <t>Intel Core i5 12400F 2.5GHz Up To 4.4GHz [Box] Socket LGA 1700</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>mdpsuperstore</t>
+          <t>Enter Komputer Official</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Palembang</t>
+          <t>Jakarta Pusat</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Rp5.699.000</t>
+          <t>Rp2.090.000</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>8 terjual</t>
+          <t>1rb+ terjual</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -506,65 +506,65 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PROCESSOR INTEL CORE I5 GEN 6 + FAN LGA / CORE I5 6600 TRAY LGA 1151</t>
+          <t>Intel Core i5 12400F Box | 4.4Ghz 6C 12T | GEN 12th LGA1700 Alder Lake</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BintangRayaKomputer</t>
+          <t>YOUNGS COMPUTER</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Kab. Sleman</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Rp590.000</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>24%</t>
-        </is>
-      </c>
+          <t>Rp1.678.000</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr">
         <is>
-          <t>15 terjual</t>
+          <t>100+ terjual</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Intel Core i5 3470 Tray + Fan</t>
+          <t>Intel Core i5-10400F LGA1200 6C/12T 4.3Ghz 12MB 65W Komputer Prosessor</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>JnJ Online</t>
+          <t>Agres Komputer Bandung</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Rp711.000</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
+          <t>Rp1.275.000</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>17%</t>
+        </is>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1 terjual</t>
+          <t>9 terjual</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -576,12 +576,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Intel Core i5 11400 TRAY 2.6GHz 6 Core 12 Threads - LGA1200</t>
+          <t>Intel Core i5 9600K - 3.7GHz 6-Core (Socket 1151 Coffe Lake Gen 9)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>JnJ Online</t>
+          <t>Toko Expert Komputer</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -591,13 +591,13 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Rp2.439.000</t>
+          <t>Rp3.938.000</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr">
         <is>
-          <t>23 terjual</t>
+          <t>30+ terjual</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -609,28 +609,32 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Intel Core i5 10400 2.9GHz 6 Core 12 Thread Comet Lake - LGA1200</t>
+          <t>Intel Core i5-14400F LGA1700 6P+4E/16T 4.7Ghz 20MB 65W Komputer Prosessor</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>JnJ Online</t>
+          <t>Agres Komputer Bandung</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Rp2.299.000</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr"/>
+          <t>Rp2.190.000</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>52%</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>250+ terjual</t>
+          <t>30+ terjual</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -642,61 +646,61 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Intel core i5 7400 3.0 GHz Tray + FAN - LGA1151</t>
+          <t>INTEL PROCESSOR CORE I5 13400F - LGA1700</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>JnJ Online</t>
+          <t>Ramai Cell26</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Surabaya</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Rp1.472.000</t>
+          <t>Rp920.000</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr">
         <is>
-          <t>3 terjual</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
+          <t>5 terjual</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Intel Core i5 14400F 10 Core 16 Thread Up To 4.7Ghz LGA 1700</t>
+          <t>Intel Core i5-13400F LGA1700 6P+4E/16T 4.6Ghz 20MB 65W Komputer Prosessor</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Starcomp Purwokerto</t>
+          <t>Agres Komputer Bandung</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Kab. Banyumas</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Rp2.549.000</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
+          <t>Rp1.950.000</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>14%</t>
+        </is>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>1 terjual</t>
+          <t>30+ terjual</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -708,12 +712,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Intel Core i5-760 Processor 8M Cache, 2.80 GHz</t>
+          <t>PROCESSOR INTEL CORE I5 12400F 4.40 GHz BOX SOCKET 1700 3 TAHUN</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>JnJ Online</t>
+          <t>QueenProcessor</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -723,46 +727,50 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Rp1.117.000</t>
+          <t>Rp1.988.001</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1 terjual</t>
+          <t>2rb+ terjual</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Intel Core i5 11400F 2.6GHz 6 Core 12 Threads Rocket Lake - LGA1200</t>
+          <t>INTEL PROCESSOR I5 12400F LGA1700 - PROCESSOR INTEL - PROCESSOR INTEL I5 - PROCESSOR LGA 1700 - I5 GEN 12</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>JnJ Online</t>
+          <t>Agres Komputer Official</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Jakarta Utara</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Rp2.129.000</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
+          <t>Rp1.940.000</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>39%</t>
+        </is>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>50+ terjual</t>
+          <t>250+ terjual</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -774,28 +782,28 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Intel Core i5 4590 3.3Ghz Socket LGA 1150 Haswell Intel Gen 4 Tray</t>
+          <t>Paket Processor Gaming Intel Core i5 14400F Box Gen 14 LGA 1700 RAM DDR5 32GB</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Starcomp Purwokerto</t>
+          <t>Mandiri Teknologi_NEW</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Kab. Banyumas</t>
+          <t>Jakarta Utara</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Rp402.000</t>
+          <t>Rp6.475.000</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>3 terjual</t>
+          <t>1 terjual</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -807,28 +815,28 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Intel Core i5 10400F 2.9GHz 6 Core 12 Thread Comet Lake - LGA1200</t>
+          <t>Processor Intel Core i5 4570 / 4590 / 4670 / 4690 Tray Socket 1150 Ci5</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>JnJ Online</t>
+          <t>Panda PC</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Kab. Tangerang</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Rp1.679.000</t>
+          <t>Rp272.000</t>
         </is>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>500+ terjual</t>
+          <t>5rb+ terjual</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -840,32 +848,28 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Processor CPU Intel Core i5-4590 | 4 Cores | 3.70 GHz 6MB Cache | Intel HD Graphics 4600 | LGA1150 | TDP 84W | Tray Garansi 1 Tahun</t>
+          <t>Intel Core i5 8500 Tray + Fan Coffe lake - Intel LGA 1151 H110</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>UV Computer Mall</t>
+          <t>Cheap n Cheap</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Medan</t>
+          <t>Denpasar</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Rp349.000</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2%</t>
-        </is>
-      </c>
+          <t>Rp274.000</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr">
         <is>
-          <t>11 terjual</t>
+          <t>4 terjual</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -877,28 +881,28 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Intel Core i5 12400F 2.5GHz Up To 4.4GHz Socket LGA 1700</t>
+          <t>Intel Core i5-11400F 2.6Ghz Up To 4.4Ghz [Tray] LGA 1200</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Starcomp Semarang</t>
+          <t>Enter Komputer Official</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Semarang</t>
+          <t>Jakarta Pusat</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Rp1.899.000</t>
+          <t>Rp1.229.000</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr">
         <is>
-          <t>30+ terjual</t>
+          <t>40+ terjual</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -910,32 +914,28 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Intel Core i5-12400F Processor CPU Gen 12 Alder Lake LGA1700 LGA-1700 TRAY Garansi 1 Tahun</t>
+          <t>Intel Core i5 3470 3.60GHz+ Fan 1155</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>UV Computer Mall</t>
+          <t>Pc Murah Comp</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Medan</t>
+          <t>Bekasi</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Rp1.749.000</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
+          <t>Rp249.800</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
       <c r="F15" t="inlineStr">
         <is>
-          <t>11 terjual</t>
+          <t>500+ terjual</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -947,32 +947,28 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Processor CPU Intel Core i5-4570 | 4 Cores | 3.60 GHz 6MB Cache | Intel HD Graphics 4600 | LGA1150 | TDP 84W | Tray Garansi 1 Tahun</t>
+          <t>Intel Core i5 12400F BOX (INTEL LGA 1700)</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>UV Computer Mall</t>
+          <t>Toko Expert Komputer</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Medan</t>
+          <t>Jakarta Pusat</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Rp329.000</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>6%</t>
-        </is>
-      </c>
+          <t>Rp2.010.000</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr">
         <is>
-          <t>2 terjual</t>
+          <t>1rb+ terjual</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -984,28 +980,28 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Intel Core i5 10400 2.9 GHz BOX Socket LGA1200 CPU Processor</t>
+          <t>Processor Intel Core i5 13400F 2.5GHz Up To 4.6GHz - [Box] LGA 1700</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Starcomp Semarang</t>
+          <t>Enter Komputer Official</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Semarang</t>
+          <t>Jakarta Pusat</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Rp2.150.000</t>
+          <t>Rp2.320.000</t>
         </is>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="inlineStr">
         <is>
-          <t>11 terjual</t>
+          <t>250+ terjual</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1017,28 +1013,32 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Intel Core i5-12400F Processor CPU Gen 12 Alder Lake LGA1700 LGA-1700 Box Garansi Resmi 3 Tahun</t>
+          <t>INTEL PROCESSOR I5 12400F LGA1700 1YT - PROCESSOR INTEL I5 GEN 12 - PROCESSOR INTEL GEN 12 - INTEL I5 12400F</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>UV Computer Mall</t>
+          <t>Agres Komputer Official</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Medan</t>
+          <t>Jakarta Utara</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Rp2.190.000</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
+          <t>Rp1.637.000</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>36%</t>
+        </is>
+      </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>29 terjual</t>
+          <t>100+ terjual</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1050,28 +1050,28 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Intel Core i5 12400 2.5GHz Up To 4.4GHz Socket LGA 1700 BOX</t>
+          <t>INTEL CORE I5 12400F | Desktop Processor Gen 12 LGA 1700</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Starcomp Semarang</t>
+          <t>Lezz Computech</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Semarang</t>
+          <t>Jakarta Utara</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Rp2.499.000</t>
+          <t>Rp1.749.000</t>
         </is>
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="inlineStr">
         <is>
-          <t>24 terjual</t>
+          <t>30+ terjual</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1083,28 +1083,28 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Processor CPU Intel Core i5-3470 | 4 Cores | 3.60 GHz 6MB Cache | Intel HD Graphics 2500 | LGA1155 | TDP 77W | Tray Garansi 1 Tahun</t>
+          <t>Intel Core i5-14400F</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>UV Computer Mall</t>
+          <t>COC Komputer</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Medan</t>
+          <t>Jakarta Pusat</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Rp295.000</t>
+          <t>Rp2.625.000</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="inlineStr">
         <is>
-          <t>3 terjual</t>
+          <t>100+ terjual</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1116,28 +1116,28 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Processor Intel Core i5-12400F Up To 4.4GHz Socket LGA 1700 Alder Lake</t>
+          <t>Intel Core i5-10400F 2.9Ghz Up To 4.3Ghz - Cache 12MB [Box] LGA 1200</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ESES Komputer Tasikmalaya</t>
+          <t>Enter Komputer Official</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Tasikmalaya</t>
+          <t>Jakarta Pusat</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Rp2.056.000</t>
+          <t>Rp1.699.000</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr">
         <is>
-          <t>22 terjual</t>
+          <t>1rb+ terjual</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1149,28 +1149,28 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Processor CPU Intel Core i5-10400 | 6 Cores | 4.30 GHz 12MB Cache | Intel UHD Graphics 630 | LGA1200 | TDP 65W | Box Garansi 3 Tahun</t>
+          <t>Processor Intel Core i5-14600K 3.5GHz Up To 5.3GHz - [Box] LGA 1700</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>UV Computer Mall</t>
+          <t>Enter Komputer Official</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Medan</t>
+          <t>Jakarta Pusat</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Rp2.150.000</t>
+          <t>Rp4.079.000</t>
         </is>
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="inlineStr">
         <is>
-          <t>2 terjual</t>
+          <t>60+ terjual</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1182,28 +1182,28 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Intel Core i5 13400F 2.5GHz Up To 4.6GHz LGA 1700 CPU Processor</t>
+          <t>PAKET Intel Core I5 10400F (Gen 10) TRAY + Motherboard MSI H510 DDR4 Socket LGA 1200</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Starcomp Semarang</t>
+          <t>Cahaya Komputer ID</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Semarang</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Rp2.379.000</t>
+          <t>Rp1.375.000</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr">
         <is>
-          <t>6 terjual</t>
+          <t>2 terjual</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1215,28 +1215,28 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Processor CPU Intel Core i5-10400F | 6 Cores | 4.30 GHz 12MB Cache | Tanpa Intel UHD | LGA1200 | TDP 65W | Box Garansi 3 Tahun</t>
+          <t>Processor Intel Core i5 12400F LGA 1700</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>UV Computer Mall</t>
+          <t>ITShop Online</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Medan</t>
+          <t>Surabaya</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Rp1.710.000</t>
+          <t>Rp2.300.000</t>
         </is>
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="inlineStr">
         <is>
-          <t>2 terjual</t>
+          <t>1rb+ terjual</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1248,28 +1248,32 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Intel Core i5-14400F 10 Core 16 Thread Up To 4.7Ghz LGA 1700</t>
+          <t>Intel Core i5-14400 LGA1700 6P+4E/16T 4.7Ghz UHD730 20MB 65W</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Starcomp Semarang</t>
+          <t>Agres Komputer Bandung</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Semarang</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Rp2.549.000</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr"/>
+          <t>Rp2.550.000</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>49%</t>
+        </is>
+      </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>11 terjual</t>
+          <t>6 terjual</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1281,82 +1285,70 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Processor CPU Intel Core i5-12400 | 6 Cores | 4.40 GHz 18MB Cache |  Intel UHD Graphics 730 | LGA1700 | TDP 65W | TRAY Garansi 1 Tahun</t>
+          <t>Intel Core i5 10400F - 2.9GHz 6 Core Comet Lake - LGA1200</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>UV Computer Mall</t>
+          <t>DCS Komputer_NEW</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Medan</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Rp2.299.000</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>5%</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>8 terjual</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
+          <t>Rp1.610.000</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Intel Core i5-13400F - 10 Core 16 Threads 4.60GHz</t>
+          <t>PC Rakitan Intel Core i5 12400 gen 12 | ssd nvme | ram 8/16gb</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Julyaugustshop</t>
+          <t>POINT99 COMPUTER</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Rp2.300.000</t>
+          <t>Rp4.675.000</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
-          <t>25 terjual</t>
+          <t>70+ terjual</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.8</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Intel Core i5 10400 TRAY FAN - 2.9GHz 6 Core 12 Thread LGA1200</t>
+          <t>ADVAN Workpro Intel Core i5 12450H RAM32GB SSD1TB 14'' FHD IPS  Windows 11</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Julyaugustshop</t>
+          <t>SKYTECH STORE ID</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1366,30 +1358,30 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Rp1.850.000</t>
+          <t>Rp5.349.000</t>
         </is>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr">
         <is>
-          <t>1 terjual</t>
+          <t>60+ terjual</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Intel Core i5 12400 - 6 cores 12 threads up to 4.4 GHz</t>
+          <t>Processor Intel Core i5 13400F 10 Core 16 Threads 4.60GHz (LGA 1700)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Julyaugustshop</t>
+          <t>Toko Expert Komputer</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1399,13 +1391,13 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Rp2.600.000</t>
+          <t>Rp2.338.000</t>
         </is>
       </c>
       <c r="E29" t="inlineStr"/>
       <c r="F29" t="inlineStr">
         <is>
-          <t>3 terjual</t>
+          <t>250+ terjual</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1417,12 +1409,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Intel Core i5 12400F - 6 cores 12 threads up to 4.4 GHz</t>
+          <t>INTEL CORE I5 12400F | Desktop Processor 6 (6P+0E) Cores LGA 1700</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Julyaugustshop</t>
+          <t>Nano Komputer</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1432,13 +1424,13 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Rp1.900.000</t>
+          <t>Rp2.279.000</t>
         </is>
       </c>
       <c r="E30" t="inlineStr"/>
       <c r="F30" t="inlineStr">
         <is>
-          <t>30+ terjual</t>
+          <t>750+ terjual</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1450,61 +1442,53 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Intel Core i5-11500 - 6 Core 12 Threads up To 4.6 Ghz - Gen 11 New</t>
+          <t>Processor Intel Core I5 12400F Box Alder Lake Socket LGA 1700</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Julyaugustshop</t>
+          <t>DCS Komputer_NEW</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Rp3.700.000</t>
+          <t>Rp2.120.824</t>
         </is>
       </c>
       <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>1 terjual</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Intel Core i5-11400 - 6 Core 12 Threads up To 4.4 Ghz - Gen 11 New</t>
+          <t>Intel Processor Core i5 14400F - LGA1700 - Intel gen14</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Julyaugustshop</t>
+          <t>ITShop Online</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Surabaya</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Rp2.250.000</t>
+          <t>Rp2.500.000</t>
         </is>
       </c>
       <c r="E32" t="inlineStr"/>
       <c r="F32" t="inlineStr">
         <is>
-          <t>3 terjual</t>
+          <t>30+ terjual</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1516,12 +1500,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Intel Core i5 4570 + Fan (Tray) - Socket LGA 1150</t>
+          <t>Intel Core i5 12400 BOX (INTEL LGA 1700)</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Julyaugustshop</t>
+          <t>Toko Expert Komputer</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1531,13 +1515,13 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Rp680.000</t>
+          <t>Rp2.620.000</t>
         </is>
       </c>
       <c r="E33" t="inlineStr"/>
       <c r="F33" t="inlineStr">
         <is>
-          <t>1 terjual</t>
+          <t>500+ terjual</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1549,164 +1533,164 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Intel Core i5 10400 2.9GHz Comet Lake 6 Core 12 Thread LGA1200</t>
+          <t>ACER Mate 14 AM1 Intel Core i5 1235U 8/512GB SSD Windows 11 OHS 14" WUXGA IPS</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Julyaugustshop</t>
+          <t>Acer Authorized Store Jakarta</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Jakarta Utara</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Rp2.150.000</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr"/>
+          <t>Rp7.399.000</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>14%</t>
+        </is>
+      </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>15 terjual</t>
+          <t>60+ terjual</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Proc Intel Core i5 - 6600 (3,9Ghz) Tray non fan -sky Lake 1151</t>
+          <t>Paket Mobo i5 - Motherboard H61 ECS Lga 1155 Processor Intel Core i5-3470 Ram DDR 3 Samsung/Hynix 4GB &amp; 8GB</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>AndalasSuryaGemilang</t>
+          <t>Cybercompanycomp</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Surakarta</t>
+          <t>Jakarta Barat</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Rp615.000</t>
+          <t>Rp549.000</t>
         </is>
       </c>
       <c r="E35" t="inlineStr"/>
       <c r="F35" t="inlineStr">
         <is>
-          <t>1 terjual</t>
+          <t>70+ terjual</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.8</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>PROCESSOR INTEL CORE I5 12400F TRAY</t>
+          <t>Intel Core i5-3570 3.4Ghz Cache 6MB [Tray] Socket LGA 1155</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>RedTeknologi-Redcom</t>
+          <t>QueenProcessor</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Jakarta Barat</t>
+          <t>Jakarta Pusat</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Rp1.762.000</t>
+          <t>Rp229.001</t>
         </is>
       </c>
       <c r="E36" t="inlineStr"/>
       <c r="F36" t="inlineStr">
         <is>
-          <t>1 terjual</t>
+          <t>1rb+ terjual</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>PROCESSOR INTEL CORE I5 10400F TRAY</t>
+          <t>PROCESSOR INTEL CORE I5 7500 [TRAY+FAN] SOCKET 1151 3.4GHz</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>RedTeknologi-Redcom</t>
+          <t>QueenProcessor</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Jakarta Barat</t>
+          <t>Jakarta Pusat</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Rp1.315.500</t>
+          <t>Rp629.001</t>
         </is>
       </c>
       <c r="E37" t="inlineStr"/>
       <c r="F37" t="inlineStr">
         <is>
-          <t>1 terjual</t>
+          <t>250+ terjual</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.8</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>SPC LIFE 5 – Intel Core i5|8GB DDR4|Storage: 512GB|Garansi Resmi SPC 1 tahun</t>
+          <t>MSI Core i5 Modern 14 C12MO 9S7-14J112-1287 Black</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>SPC Indonesia</t>
+          <t>ITShop Online</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Jakarta Utara</t>
+          <t>Surabaya</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Rp5.950.000</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>54%</t>
-        </is>
-      </c>
+          <t>Rp7.000.000</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr"/>
       <c r="F38" t="inlineStr">
         <is>
-          <t>1 terjual</t>
+          <t>6 terjual</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -1718,61 +1702,65 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>INTEL CORE I5 10400 GEN 10</t>
+          <t>Laptop HP Victus 15 FA2716TX GeForce RTX 3050 - I5 13420H RAM 8GB 512GB SSD 144HZ</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>YOESTORE</t>
+          <t>NVIDIA GeForce Laptop</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Jakarta Utara</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Rp2.200.000</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr"/>
+          <t>Rp11.499.000</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>36%</t>
+        </is>
+      </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>50+ terjual</t>
+          <t>100+ terjual</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Intel Core i5 10400F 2.9GHz Comet Lake 6 Core 12 Thread LGA1200</t>
+          <t>PAKET Intel I5 12400F (Gen 12) TRAY LGA 1700 + Motherborad MSI H610 DDR4 Garansi</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Julyaugustshop</t>
+          <t>Cahaya Komputer ID</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Rp1.615.000</t>
+          <t>Rp1.795.000</t>
         </is>
       </c>
       <c r="E40" t="inlineStr"/>
       <c r="F40" t="inlineStr">
         <is>
-          <t>60+ terjual</t>
+          <t>13 terjual</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1784,28 +1772,32 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Intel Core i5 10400 2.9GHz 6 Core 12 Thread Comet Lake - LGA1200</t>
+          <t>INTEL PROCESSOR I5 14400F LGA1700 [2.50-4.70 GHz, 6C/12T, LGA 1700]</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>GX COMP</t>
+          <t>IMBA PC</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Bandung</t>
+          <t>Jakarta Utara</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Rp2.229.000</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr"/>
+          <t>Rp2.170.000</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>13%</t>
+        </is>
+      </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2 terjual</t>
+          <t>4 terjual</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -1817,28 +1809,28 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Processor Intel Core I5 13400F Box Raptor Lake Socket LGA 1700</t>
+          <t>Acer Aspire Lite 14 Core i5 1235U i3 1215U N100 16GB 512GB Win+OHS 14.0</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Jaya Pro Computer</t>
+          <t>KangLaptop_NEW</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Jakarta Selatan</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Rp2.295.000</t>
+          <t>Rp9.899.000</t>
         </is>
       </c>
       <c r="E42" t="inlineStr"/>
       <c r="F42" t="inlineStr">
         <is>
-          <t>11 terjual</t>
+          <t>13 terjual</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -1850,41 +1842,45 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Processor Intel Core i5 13400F 2.5GHz Up To 4.6GHz - [Box] LGA 1700</t>
+          <t>Paket Processor Intel Core i5 12400 / i5 12400F Box LGA 1700 Gen 12 DDR4 NVME</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>GX COMP</t>
+          <t>Mandiri Teknologi_NEW</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Bandung</t>
+          <t>Jakarta Utara</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Rp2.450.000</t>
+          <t>Rp4.350.000</t>
         </is>
       </c>
       <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr"/>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>30+ terjual</t>
+        </is>
+      </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Processor Intel Core I5 10400 Box Comet Lake Socket LGA 1200</t>
+          <t>Intel Core i5-7500 TRAY + FAN - 3.4Ghz - KabyLake Socket 1151</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Jaya Pro Computer</t>
+          <t>Toko Expert Komputer</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1894,13 +1890,13 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Rp2.094.000</t>
+          <t>Rp708.000</t>
         </is>
       </c>
       <c r="E44" t="inlineStr"/>
       <c r="F44" t="inlineStr">
         <is>
-          <t>100+ terjual</t>
+          <t>50+ terjual</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -1912,12 +1908,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Processor Intel Core I5 12400F Box Alder Lake Socket LGA 1700</t>
+          <t>Processor Intel Core I5 12400 Box Alder Lake Socket LGA 1700</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Jaya Pro Computer</t>
+          <t>Jaya PC</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1927,7 +1923,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Rp1.985.000</t>
+          <t>Rp2.555.000</t>
         </is>
       </c>
       <c r="E45" t="inlineStr"/>
@@ -1945,28 +1941,28 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Processor Intel Core I5 10400F Box Comet Lake Socket LGA 1200</t>
+          <t>Intel core i5 6500 3.20ghz</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Jaya Pro Computer</t>
+          <t>novcom</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Kab. Bogor</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Rp1.670.000</t>
+          <t>Rp444.000</t>
         </is>
       </c>
       <c r="E46" t="inlineStr"/>
       <c r="F46" t="inlineStr">
         <is>
-          <t>500+ terjual</t>
+          <t>50+ terjual</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -1978,28 +1974,28 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Processor Intel Core I5 12400 Box Alder Lake Socket LGA 1700</t>
+          <t>Intel Core i5 7500 Tray + Fan Kabylake - Intel LGA 1151 H110</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Jaya Pro Computer</t>
+          <t>Cheap n Cheap</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Denpasar</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Rp2.430.000</t>
+          <t>Rp274.000</t>
         </is>
       </c>
       <c r="E47" t="inlineStr"/>
       <c r="F47" t="inlineStr">
         <is>
-          <t>90+ terjual</t>
+          <t>1 terjual</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2011,28 +2007,32 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Promo Intel Free Gift untuk setiap pembelian minimal Intel Core i5</t>
+          <t>Intel Core I5 13400 Desktop Processor 10 Cores Upto 4.60 GHz Socket LGA1700</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Laptop Grosir ID</t>
+          <t>Gamer ID Bandung</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Jakarta Selatan</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Rp249.000</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr"/>
+          <t>Rp2.490.000</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>13%</t>
+        </is>
+      </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>19 terjual</t>
+          <t>5 terjual</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2044,28 +2044,32 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Processor Intel Core I5-12400F 2.5 GHz 6 Core 12 Threads LGA1700</t>
+          <t>PC GAMING GEN 12 INTEL CORE I5 12400F VGA NVIDIA GT 730 8GB RAM WHITE</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Tech In Store</t>
+          <t>Kadal Gaming Surabaya</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Jakarta Utara</t>
+          <t>Surabaya</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Rp1.876.000</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr"/>
+          <t>Rp4.590.000</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>21%</t>
+        </is>
+      </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>1 terjual</t>
+          <t>10 terjual</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -2077,28 +2081,28 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>PROCESSOR INTEL CORE I5 3470 TRAY + FAN</t>
+          <t>intel core i5 3470 tray lga 1155</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>KPC12</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Jakarta Utara</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Rp315.000</t>
+          <t>Rp213.000</t>
         </is>
       </c>
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>3 terjual</t>
+          <t>4rb+ terjual</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2110,28 +2114,28 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>PROCESSOR INTEL CORE I5 2400 TRAY + FAN</t>
+          <t>HP 14 Intel Core I5 Gen 13 Ram 16Gb 512Gb Win 11 Office 14 Inch Full HD IPS</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>AGRES ID Jakarta Timur</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Jakarta Timur</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Rp285.000</t>
+          <t>Rp8.349.000</t>
         </is>
       </c>
       <c r="E51" t="inlineStr"/>
       <c r="F51" t="inlineStr">
         <is>
-          <t>8 terjual</t>
+          <t>20 terjual</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2143,12 +2147,12 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Processor Intel Core i5 11500 12M Cache Up To 4.6Ghz Box Socket 1200</t>
+          <t>Intel Core I5 4570 3.2Ghz TRAY + FAN INTEL (Socket 1150)</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>Toko Expert Komputer</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2158,13 +2162,13 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Rp2.225.000</t>
+          <t>Rp343.600</t>
         </is>
       </c>
       <c r="E52" t="inlineStr"/>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2 terjual</t>
+          <t>100+ terjual</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -2176,12 +2180,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>PROCESSOR INTEL CORE I5 3570 TRAY + FAN</t>
+          <t>Lenovo LOQ 15IAX9E Essential i5 12450HX RTX3050 6GB/ 12GB 512GB W11+OHS 15.6FHD 144HZ 100SRGB</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>Lenovo Legion Official</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -2191,46 +2195,54 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Rp290.000</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr"/>
+          <t>Rp11.499.000</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>18%</t>
+        </is>
+      </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>8 terjual</t>
+          <t>100+ terjual</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Processor Intel Core i5-10400 12M Cache Up To 4.30Ghz Box Socket 1200</t>
+          <t>ACER ASPIRE 7 PRO A715 59G 56K7 I5 12450H 16GB 512GB RTX3050 6GB 15.6" FHD 144Hz OHS24  Windows</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>Acer Exclusive Pondok Indah</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Jakarta Selatan</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Rp1.865.000</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr"/>
+          <t>Rp9.899.000</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>18%</t>
+        </is>
+      </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>6 terjual</t>
+          <t>15 terjual</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2242,28 +2254,28 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>PROCESSOR INTEL CORE I5 4460 TRAY + FAN ORI</t>
+          <t>Processor Intel Core i5 12400 LGA 1700</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>ITShop Online</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Surabaya</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Rp355.000</t>
+          <t>Rp2.700.000</t>
         </is>
       </c>
       <c r="E55" t="inlineStr"/>
       <c r="F55" t="inlineStr">
         <is>
-          <t>12 terjual</t>
+          <t>750+ terjual</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2275,12 +2287,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Processor Intel Core I5 12400F Box Alder Lake - Socket LGA 1700 2.5Ghz</t>
+          <t>INTEL CORE I5 11400F 2.6GHz ROCKET LAKE 6 CORE 12 THREAD LGA1200 [BOX]</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>QueenProcessor</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2290,30 +2302,30 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Rp1.825.000</t>
+          <t>Rp1.699.001</t>
         </is>
       </c>
       <c r="E56" t="inlineStr"/>
       <c r="F56" t="inlineStr">
         <is>
-          <t>40+ terjual</t>
+          <t>1rb+ terjual</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.9</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Processor Intel Core i5 11400 12M Cache Up To 4.4Ghz Box Socket 1200</t>
+          <t>Asus Vivobook F1504ZA i5 1235u 8GB SSD 512GB IrisXe 15,6" FHD IPS Windows 11 Home</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>aura technology</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
@@ -2323,13 +2335,13 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Rp2.260.000</t>
+          <t>Rp7.099.000</t>
         </is>
       </c>
       <c r="E57" t="inlineStr"/>
       <c r="F57" t="inlineStr">
         <is>
-          <t>5 terjual</t>
+          <t>70+ terjual</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
@@ -2341,12 +2353,12 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Processor Intel Core I5 11400 Tray -6 Core 12 Threads Socket LGA 1200</t>
+          <t>INTEL CORE I5 12400 4.40 GHz BOX SOCKET 1700 3 TAHUN</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>QueenProcessor</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2356,30 +2368,30 @@
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Rp1.798.000</t>
+          <t>Rp2.499.001</t>
         </is>
       </c>
       <c r="E58" t="inlineStr"/>
       <c r="F58" t="inlineStr">
         <is>
-          <t>13 terjual</t>
+          <t>250+ terjual</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>5.0</t>
+          <t>4.8</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Processor Intel Core i5 11400F 12M Cache Up To 4.4Ghz Box Socket 1200</t>
+          <t>Asus VivoBook 15 Core I5 Gen 12 16GB 512 SSD W 11 15.6 Inch IPS Panel</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>ROGZ Online</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2389,13 +2401,13 @@
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Rp2.098.000</t>
+          <t>Rp7.499.000</t>
         </is>
       </c>
       <c r="E59" t="inlineStr"/>
       <c r="F59" t="inlineStr">
         <is>
-          <t>13 terjual</t>
+          <t>50+ terjual</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
@@ -2407,64 +2419,1911 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Processor Intel Core I5 12400 Box Alder Lake - Socket LGA 1700 2.5Ghz</t>
+          <t>Processor Intel Core i5 14600K 3.5GHz Up To 5.3GHz - [Box] LGA 1700</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>Makassar xtream computer</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Makassar</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Rp2.550.000</t>
+          <t>Rp4.500.000</t>
         </is>
       </c>
       <c r="E60" t="inlineStr"/>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>20 terjual</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Processor Intel Core I5 13400F Box - Raptor Lake Socket LGA 1700</t>
+          <t>Intel Core i5-10400 LGA 1200 gen 10</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Duta Mandiri Infokom</t>
+          <t>WB Computer</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Jakarta Pusat</t>
+          <t>Bandung</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Rp2.275.000</t>
+          <t>Rp1.695.000</t>
         </is>
       </c>
       <c r="E61" t="inlineStr"/>
       <c r="F61" t="inlineStr">
         <is>
-          <t>5 terjual</t>
+          <t>12 terjual</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Intel Core i5 12400 2.5 GHz 6 Core 12 Threads Alder Lake LGA1700</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>ONE IT EXPERT</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>Surabaya</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Rp2.923.000</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>60+ terjual</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>PC / CPU / KOMPUTER RAKITAN CORE i5 BARU GARANSI 1 TAHUN</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>NENET COMPUTER</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>Bandung</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Rp1.400.000</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>1rb+ terjual</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Processor Intel Core i5 - 4590 3.5Ghz Tray + Fan Socket 1150</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>QueenProcessor</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Rp319.001</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>1rb+ terjual</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Intel Core i5 12400 2.5GHz Up To 4.4GHz [Box] Socket LGA 1700</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>XFun Gaming</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Samarinda</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Rp2.400.000</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Intel Core i5-10400 2.9Ghz Up To 4.3Ghz - Cache 12 MB [Box] LGA 1200</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Enter Komputer Official</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Rp2.169.000</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>250+ terjual</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Paketan Intel Core i5 14400F with Motherboard LGA 1700 MSI Ram DDR4 or Mobo not Ryzen - PAKETAN CPU</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>alat gaming77</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>Medan</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Rp2.255.000</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>45%</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>1 terjual</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr"/>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Paket Processor Gaming Intel Core i5 12400F Box Gen 12 LGA 1700 B660 RAM DDR4 16GB RGB</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Mandiri Teknologi_NEW</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>Jakarta Utara</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Rp4.850.000</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>2 terjual</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Intel Core i5 12400F 2.5GHz Up To 4.4GHz Socket LGA 1700</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Starcomp Semarang</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Rp2.165.000</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>40+ terjual</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Intel Core i5 12400 2.5GHz Up To 4.4GHz Socket LGA 1700 BOX</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Starcomp Semarang</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>Semarang</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Rp2.690.000</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>24 terjual</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>PROC INTEL CORE - i5 11400F ROCKET LAKE include fan (Harus pasang Vga) (BX8070811400F)</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Maha.Gadget</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>Kab. Tabanan</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Rp1.815.000</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>PROCESSOR INTEL CORE I5 12500 BOX 4.60 GHz BOX SOCKET 1700 3 TAHUN</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>QueenProcessor</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Rp3.299.001</t>
+        </is>
+      </c>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>80+ terjual</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Intel core i5 6500 3.20ghz</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>novcom</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>Kab. Bogor</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Rp445.000</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>ACER ASPIRE LITE AL14-71P I5 13500H 16GB 512GB W11+OHS 14.0WUXGA IPS</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>AGRES ID</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>Jakarta Utara</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Rp8.309.000</t>
+        </is>
+      </c>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>26%</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>100+ terjual</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Paketan Asrock B560M Pro 4 i5 10400f Normal Bekas Pemakaian Pribadi Bundle Mobo Intel LGA 1200</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>Tekdino</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>Tangerang Selatan</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Rp2.650.000</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Processor Intel Core I5 12400 Box Alder Lake Socket LGA 1700</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>Jaya Pro Computer</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Rp2.550.000</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>90+ terjual</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Processor Intel Core i5 10400 Comet Lake</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>Blessing Computer Bali</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>Denpasar</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Rp2.109.000</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>100+ terjual</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Processor Intel Core i5 12400F Alder Lake LGA1700 Harus Pasang VGA</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>Blessing Computer Bali</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Denpasar</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Rp2.199.000</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>250+ terjual</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>PROCESSOR INTEL CORE I5 12400 4.40 GHz BOX SOCKET 1700 3 TAHUN</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>QueenProcessor</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Rp2.499.001</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>1rb+ terjual</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Cpu intel core i5 13400</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>Berau Komp</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>Kab. Berau</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Rp3.000.000</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Intel Core i5 14400 Box Up To 4.7Ghz 10 Core 16 Thread LGA 1700 Gen 14th</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>YOUNGS COMPUTER</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>Kab. Sleman</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Rp2.728.000</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>11 terjual</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>3.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>INTEL CORE I5 11600K Processor Intel Gen 11 LGA 1200 6 Core</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>Ssynergy.id</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>Bandar Lampung</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>Rp4.849.000</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>PC Gaming Gen 12 | i5 12400F | RTX 4060 8GB | 16GB DDR4 | NVME |Render</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>Venom Gaming Store Official</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>Kab. Tangerang</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>Rp10.625.000</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr"/>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>100+ terjual</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Intel Core i5 10400F 2.9GHz 6 Core (Intel LGA 1200, Gen 10)</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>Toko Expert Komputer</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Rp1.705.000</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>250+ terjual</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Promo Processor Intel Core i5-14400F up to 4.7GHz Box LGA 1700</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>Aska Sttore</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>Rp1.917.000</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Processor Intel core i5 6500 3.2 GHz TRAY + FAN Socket 1151</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>QueenProcessor</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>Rp499.001</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr"/>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>1rb+ terjual</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Acer Nitro V15 ANV15-51-5430 with Intel i5-13420H and NVIDIA RTX4050 AND 16GB DDR5</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>TEKNO ELEKTRONIK SHOP</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>Jakarta Selatan</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>Rp7.012.500</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>45%</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>7 terjual</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr"/>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Processor Intel Core I5 11400F (LGA 1200 Gen 11)</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Toko Expert Komputer</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>Rp1.712.000</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>250+ terjual</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Prosesor Intel Core i5-10400 (Cache 12M, hingga 4,30 GHz)</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Angelina Computer_NEW</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>Surabaya</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>Rp2.700.000</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>50+ terjual</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Processor Intel Core i5 12400 2.5 GHz 6 Core Alder Lake LGA 1700 New</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Mugen Computer</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>Makassar</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>Rp2.625.000</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr"/>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>1 terjual</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr"/>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Intel Core i5 4590 Tray + Fan - Intel LGA 1150 H81</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>Cheap n Cheap</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Denpasar</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>Rp161.000</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr"/>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>25 terjual</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Core i5 9400F 4.1GHz Gen 9 Processor Intel 1151 Coffeelakes</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>Najch Creative House</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Kab. Cirebon</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>Rp999.500</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr"/>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>10 terjual</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>INTEL CORE I5 12400F | GEN 12 LGA 1700 TRAY</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>PC Rakitan Official</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>Jakarta Utara</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>Rp1.637.000</t>
+        </is>
+      </c>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>3%</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>6 terjual</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr"/>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>INTEL PROCESSOR I5 12600K LGA1700 3Y</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>Agres Komputer Official</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>Jakarta Utara</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>Rp2.760.000</t>
+        </is>
+      </c>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>35%</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Cpu intel core i5 Ram8gb</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>redy allshop</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>Medan</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>Rp4.000.000</t>
+        </is>
+      </c>
+      <c r="E95" t="inlineStr"/>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>8 terjual</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>Intel Core i5 10400F | Processor Gen 10 Comet Lake LGA 1200</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>Lezz Computech</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>Jakarta Utara</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>Rp1.349.000</t>
+        </is>
+      </c>
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>14 terjual</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Paket PC Intel Core I5 4590</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>Kita Computer.</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>Mataram</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>Rp6.200.000</t>
+        </is>
+      </c>
+      <c r="E97" t="inlineStr"/>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr"/>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Processor INTEL CORE i5 14400 (LGA 1700)</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>Toko Expert Komputer</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>Rp3.370.000</t>
+        </is>
+      </c>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>18 terjual</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>4.7</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>Paket Processor Intel i5 13400 / i5 13400F Tray Gen 13 LGA 1700 DDR5</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>Mandiri Teknologi_NEW</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>Jakarta Utara</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>Rp5.050.000</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>1 terjual</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr"/>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>PROCESSOR INTEL CORE I5 13400F 4.60 GHz BOX SOCKET 1700 GARANSI 3TAHUN</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>QueenProcessor</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>Rp2.299.001</t>
+        </is>
+      </c>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>250+ terjual</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Processor Intel Core I5 14400F Box Raptor Lake Socket LGA 1700</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>Jaya PC</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>Rp3.220.000</t>
+        </is>
+      </c>
+      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>25 terjual</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Intel i5 4590 up to 3.70GHz</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>PGNet Computer</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>Kab. Bogor</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Rp280.000</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>100+ terjual</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Intel I5 11400F + H510M Pro</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>Hanareta</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>Kab. Bantul</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Rp1.300.000</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Intel Core i5 9600K Coffee Lake 6-Core 3.7 GHz LGA 1151</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>Mega Surya Computer_NEW</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>Banjarmasin</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Rp3.053.987</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Processor Intel Core I5 12400F Box Alder Lake Socket LGA 1700</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>Jaya PC</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Rp1.990.000</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>250+ terjual</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Intel Core i5 10400F - Socket LGA 1200 [TRAY]</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>Persada Computer</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>Bandung</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Rp1.270.000</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>80+ terjual</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Processor Intel Core I5 12400 Box Alder Lake Socket LGA 1700</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>Raja Harddisk</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Rp2.550.000</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>10 terjual</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Intel Core i5-10400F</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>COC Komputer</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Rp1.710.000</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>80+ terjual</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>INTEL PROCESSOR I5 12400F LGA1700 3Y  BOX</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>Gamer Rakitan</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Rp1.960.000</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr"/>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>PROCESSOR INTEL CORE I5 12400F 4.40 GHz TRAY SOCKET 1700</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>QueenProcessor</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Rp1.699.001</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>1rb+ terjual</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>INTEL PROCESSOR I5 12400F LGA1700 1YT</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>PC Rakitan Official</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>Jakarta Utara</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Rp1.637.000</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>5%</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>100+ terjual</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>4.8</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Intel Core i5 13500 | CPU LGA 1700</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>PGNet Computer</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Kab. Bogor</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Rp2.750.000</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr"/>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>2 terjual</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>MINI PC MSI i5 GEN 12 +WIN 11 | MSI CUBI 5 12M | INCLUDE RAM + SSD</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>Macro computer</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Rp5.620.000</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>250+ terjual</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>HOT PROCESSOR INTEL CORE I5 13400 UP TO 4.60 GHz BOX LGA 1700</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>Knight Gaming</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>Jakarta Utara</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Rp2.900.000</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>9 terjual</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Processor Intel core i5 10400F 2.9 GHz BOX Socket 1200 NEW ITEM !!!</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>QueenProcessor</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Rp1.589.001</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>3rb+ terjual</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>4.9</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Paket Processor Intel Core i5 Gen 8 Socket LGA 1151 DDR4 NVME H310</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>Mandiri Teknologi_NEW</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Jakarta Utara</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Rp2.625.000</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>25 terjual</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>Intel Processor Core i5-10400 BOX</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>POINT99 COMPUTER</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>Bandung</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Rp2.150.000</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>80+ terjual</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>PC Gaming Intel Core i5 12400F | RTX 5070 12GB | 64GB | NVMe | Mid - High</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>Frontcomp</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Bandung</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Rp5.695.000</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>3 terjual</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>PAKET Intel Core I5 3470 (Gen 3) TRAY LGA 1155 + Motherboard H61 DDR3 + CPU Fan GARANSI</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>Cahaya Komputer ID</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>Bandung</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Rp245.500</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr"/>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>7 terjual</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Intel Core I5 11400F Box Rocket Lake Socket LGA 1200</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>MAXCOM ONLINE</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>Jakarta Pusat</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Rp1.785.009</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr"/>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>22 terjual</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
         <is>
           <t>5.0</t>
         </is>

</xml_diff>